<commit_message>
acréscimo  coluna "Quantidade Vendida" no dataset
</commit_message>
<xml_diff>
--- a/produtos_precos.xlsx
+++ b/produtos_precos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:D121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>Quantidade</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Quantidade Vendida</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -462,6 +467,9 @@
       <c r="C2" t="n">
         <v>11</v>
       </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -475,6 +483,9 @@
       <c r="C3" t="n">
         <v>12</v>
       </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -488,6 +499,9 @@
       <c r="C4" t="n">
         <v>11</v>
       </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -501,6 +515,9 @@
       <c r="C5" t="n">
         <v>13</v>
       </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -514,6 +531,9 @@
       <c r="C6" t="n">
         <v>11</v>
       </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -527,6 +547,9 @@
       <c r="C7" t="n">
         <v>11</v>
       </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -540,6 +563,9 @@
       <c r="C8" t="n">
         <v>11</v>
       </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -553,6 +579,9 @@
       <c r="C9" t="n">
         <v>14</v>
       </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -566,6 +595,9 @@
       <c r="C10" t="n">
         <v>11</v>
       </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -579,6 +611,9 @@
       <c r="C11" t="n">
         <v>11</v>
       </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -592,6 +627,9 @@
       <c r="C12" t="n">
         <v>15</v>
       </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -605,6 +643,9 @@
       <c r="C13" t="n">
         <v>11</v>
       </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -618,6 +659,9 @@
       <c r="C14" t="n">
         <v>12</v>
       </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -631,6 +675,9 @@
       <c r="C15" t="n">
         <v>12</v>
       </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -644,6 +691,9 @@
       <c r="C16" t="n">
         <v>11</v>
       </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -657,6 +707,9 @@
       <c r="C17" t="n">
         <v>12</v>
       </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -670,6 +723,9 @@
       <c r="C18" t="n">
         <v>11</v>
       </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -683,6 +739,9 @@
       <c r="C19" t="n">
         <v>14</v>
       </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -696,6 +755,9 @@
       <c r="C20" t="n">
         <v>12</v>
       </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -709,6 +771,9 @@
       <c r="C21" t="n">
         <v>12</v>
       </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -722,6 +787,9 @@
       <c r="C22" t="n">
         <v>11</v>
       </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -735,6 +803,9 @@
       <c r="C23" t="n">
         <v>12</v>
       </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -748,6 +819,9 @@
       <c r="C24" t="n">
         <v>11</v>
       </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -761,6 +835,9 @@
       <c r="C25" t="n">
         <v>11</v>
       </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -774,6 +851,9 @@
       <c r="C26" t="n">
         <v>12</v>
       </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -787,6 +867,9 @@
       <c r="C27" t="n">
         <v>12</v>
       </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -800,6 +883,9 @@
       <c r="C28" t="n">
         <v>13</v>
       </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -813,6 +899,9 @@
       <c r="C29" t="n">
         <v>12</v>
       </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -826,6 +915,9 @@
       <c r="C30" t="n">
         <v>11</v>
       </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -839,6 +931,9 @@
       <c r="C31" t="n">
         <v>12</v>
       </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -852,6 +947,9 @@
       <c r="C32" t="n">
         <v>14</v>
       </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -865,6 +963,9 @@
       <c r="C33" t="n">
         <v>13</v>
       </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -878,6 +979,9 @@
       <c r="C34" t="n">
         <v>13</v>
       </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -891,6 +995,9 @@
       <c r="C35" t="n">
         <v>11</v>
       </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -904,6 +1011,9 @@
       <c r="C36" t="n">
         <v>11</v>
       </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -917,6 +1027,9 @@
       <c r="C37" t="n">
         <v>11</v>
       </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -930,6 +1043,9 @@
       <c r="C38" t="n">
         <v>13</v>
       </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -943,6 +1059,9 @@
       <c r="C39" t="n">
         <v>11</v>
       </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -956,6 +1075,9 @@
       <c r="C40" t="n">
         <v>12</v>
       </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -969,6 +1091,9 @@
       <c r="C41" t="n">
         <v>12</v>
       </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -982,6 +1107,9 @@
       <c r="C42" t="n">
         <v>11</v>
       </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -995,6 +1123,9 @@
       <c r="C43" t="n">
         <v>11</v>
       </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1008,6 +1139,9 @@
       <c r="C44" t="n">
         <v>11</v>
       </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1021,6 +1155,9 @@
       <c r="C45" t="n">
         <v>11</v>
       </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1034,6 +1171,9 @@
       <c r="C46" t="n">
         <v>11</v>
       </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1047,6 +1187,9 @@
       <c r="C47" t="n">
         <v>11</v>
       </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1060,6 +1203,9 @@
       <c r="C48" t="n">
         <v>11</v>
       </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1073,6 +1219,9 @@
       <c r="C49" t="n">
         <v>11</v>
       </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1086,6 +1235,9 @@
       <c r="C50" t="n">
         <v>12</v>
       </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1099,6 +1251,9 @@
       <c r="C51" t="n">
         <v>13</v>
       </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1112,6 +1267,9 @@
       <c r="C52" t="n">
         <v>11</v>
       </c>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1125,6 +1283,9 @@
       <c r="C53" t="n">
         <v>11</v>
       </c>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1138,6 +1299,9 @@
       <c r="C54" t="n">
         <v>14</v>
       </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1151,6 +1315,9 @@
       <c r="C55" t="n">
         <v>11</v>
       </c>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1164,6 +1331,9 @@
       <c r="C56" t="n">
         <v>15</v>
       </c>
+      <c r="D56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1177,6 +1347,9 @@
       <c r="C57" t="n">
         <v>12</v>
       </c>
+      <c r="D57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1190,6 +1363,9 @@
       <c r="C58" t="n">
         <v>13</v>
       </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1203,6 +1379,9 @@
       <c r="C59" t="n">
         <v>11</v>
       </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1216,6 +1395,9 @@
       <c r="C60" t="n">
         <v>13</v>
       </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1229,6 +1411,9 @@
       <c r="C61" t="n">
         <v>11</v>
       </c>
+      <c r="D61" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1242,6 +1427,9 @@
       <c r="C62" t="n">
         <v>14</v>
       </c>
+      <c r="D62" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1255,6 +1443,9 @@
       <c r="C63" t="n">
         <v>11</v>
       </c>
+      <c r="D63" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1268,6 +1459,9 @@
       <c r="C64" t="n">
         <v>13</v>
       </c>
+      <c r="D64" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1281,6 +1475,9 @@
       <c r="C65" t="n">
         <v>11</v>
       </c>
+      <c r="D65" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1294,6 +1491,9 @@
       <c r="C66" t="n">
         <v>12</v>
       </c>
+      <c r="D66" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1307,6 +1507,9 @@
       <c r="C67" t="n">
         <v>12</v>
       </c>
+      <c r="D67" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1320,6 +1523,9 @@
       <c r="C68" t="n">
         <v>11</v>
       </c>
+      <c r="D68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1333,6 +1539,9 @@
       <c r="C69" t="n">
         <v>12</v>
       </c>
+      <c r="D69" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1346,6 +1555,9 @@
       <c r="C70" t="n">
         <v>15</v>
       </c>
+      <c r="D70" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1359,6 +1571,9 @@
       <c r="C71" t="n">
         <v>11</v>
       </c>
+      <c r="D71" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1372,6 +1587,9 @@
       <c r="C72" t="n">
         <v>11</v>
       </c>
+      <c r="D72" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1385,6 +1603,9 @@
       <c r="C73" t="n">
         <v>11</v>
       </c>
+      <c r="D73" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1398,6 +1619,9 @@
       <c r="C74" t="n">
         <v>14</v>
       </c>
+      <c r="D74" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1411,6 +1635,9 @@
       <c r="C75" t="n">
         <v>12</v>
       </c>
+      <c r="D75" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1424,6 +1651,9 @@
       <c r="C76" t="n">
         <v>15</v>
       </c>
+      <c r="D76" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1437,6 +1667,9 @@
       <c r="C77" t="n">
         <v>14</v>
       </c>
+      <c r="D77" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1450,6 +1683,9 @@
       <c r="C78" t="n">
         <v>11</v>
       </c>
+      <c r="D78" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1463,6 +1699,9 @@
       <c r="C79" t="n">
         <v>14</v>
       </c>
+      <c r="D79" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1476,6 +1715,9 @@
       <c r="C80" t="n">
         <v>12</v>
       </c>
+      <c r="D80" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1489,6 +1731,9 @@
       <c r="C81" t="n">
         <v>12</v>
       </c>
+      <c r="D81" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1502,6 +1747,9 @@
       <c r="C82" t="n">
         <v>12</v>
       </c>
+      <c r="D82" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1515,6 +1763,9 @@
       <c r="C83" t="n">
         <v>12</v>
       </c>
+      <c r="D83" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1528,6 +1779,9 @@
       <c r="C84" t="n">
         <v>13</v>
       </c>
+      <c r="D84" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1541,6 +1795,9 @@
       <c r="C85" t="n">
         <v>11</v>
       </c>
+      <c r="D85" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -1554,6 +1811,9 @@
       <c r="C86" t="n">
         <v>11</v>
       </c>
+      <c r="D86" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -1567,6 +1827,9 @@
       <c r="C87" t="n">
         <v>11</v>
       </c>
+      <c r="D87" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -1580,6 +1843,9 @@
       <c r="C88" t="n">
         <v>12</v>
       </c>
+      <c r="D88" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -1593,6 +1859,9 @@
       <c r="C89" t="n">
         <v>11</v>
       </c>
+      <c r="D89" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -1606,6 +1875,9 @@
       <c r="C90" t="n">
         <v>14</v>
       </c>
+      <c r="D90" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -1619,6 +1891,9 @@
       <c r="C91" t="n">
         <v>13</v>
       </c>
+      <c r="D91" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -1632,6 +1907,9 @@
       <c r="C92" t="n">
         <v>12</v>
       </c>
+      <c r="D92" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -1645,6 +1923,9 @@
       <c r="C93" t="n">
         <v>15</v>
       </c>
+      <c r="D93" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -1658,6 +1939,9 @@
       <c r="C94" t="n">
         <v>12</v>
       </c>
+      <c r="D94" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -1671,6 +1955,9 @@
       <c r="C95" t="n">
         <v>12</v>
       </c>
+      <c r="D95" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -1684,6 +1971,9 @@
       <c r="C96" t="n">
         <v>12</v>
       </c>
+      <c r="D96" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -1697,6 +1987,9 @@
       <c r="C97" t="n">
         <v>13</v>
       </c>
+      <c r="D97" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -1710,6 +2003,9 @@
       <c r="C98" t="n">
         <v>11</v>
       </c>
+      <c r="D98" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -1723,6 +2019,9 @@
       <c r="C99" t="n">
         <v>12</v>
       </c>
+      <c r="D99" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -1736,6 +2035,9 @@
       <c r="C100" t="n">
         <v>11</v>
       </c>
+      <c r="D100" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -1749,6 +2051,9 @@
       <c r="C101" t="n">
         <v>11</v>
       </c>
+      <c r="D101" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -1762,6 +2067,9 @@
       <c r="C102" t="n">
         <v>11</v>
       </c>
+      <c r="D102" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -1775,6 +2083,9 @@
       <c r="C103" t="n">
         <v>13</v>
       </c>
+      <c r="D103" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -1788,6 +2099,9 @@
       <c r="C104" t="n">
         <v>13</v>
       </c>
+      <c r="D104" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -1801,6 +2115,9 @@
       <c r="C105" t="n">
         <v>13</v>
       </c>
+      <c r="D105" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -1814,6 +2131,9 @@
       <c r="C106" t="n">
         <v>12</v>
       </c>
+      <c r="D106" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -1827,6 +2147,9 @@
       <c r="C107" t="n">
         <v>13</v>
       </c>
+      <c r="D107" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -1840,6 +2163,9 @@
       <c r="C108" t="n">
         <v>13</v>
       </c>
+      <c r="D108" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -1853,6 +2179,9 @@
       <c r="C109" t="n">
         <v>15</v>
       </c>
+      <c r="D109" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -1866,6 +2195,9 @@
       <c r="C110" t="n">
         <v>12</v>
       </c>
+      <c r="D110" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -1879,6 +2211,9 @@
       <c r="C111" t="n">
         <v>13</v>
       </c>
+      <c r="D111" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -1892,6 +2227,9 @@
       <c r="C112" t="n">
         <v>13</v>
       </c>
+      <c r="D112" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -1905,6 +2243,9 @@
       <c r="C113" t="n">
         <v>11</v>
       </c>
+      <c r="D113" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -1918,6 +2259,9 @@
       <c r="C114" t="n">
         <v>11</v>
       </c>
+      <c r="D114" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -1931,6 +2275,9 @@
       <c r="C115" t="n">
         <v>12</v>
       </c>
+      <c r="D115" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -1944,6 +2291,9 @@
       <c r="C116" t="n">
         <v>11</v>
       </c>
+      <c r="D116" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -1957,6 +2307,9 @@
       <c r="C117" t="n">
         <v>11</v>
       </c>
+      <c r="D117" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -1970,6 +2323,9 @@
       <c r="C118" t="n">
         <v>13</v>
       </c>
+      <c r="D118" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -1983,6 +2339,9 @@
       <c r="C119" t="n">
         <v>11</v>
       </c>
+      <c r="D119" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -1996,6 +2355,9 @@
       <c r="C120" t="n">
         <v>12</v>
       </c>
+      <c r="D120" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -2008,6 +2370,9 @@
       </c>
       <c r="C121" t="n">
         <v>13</v>
+      </c>
+      <c r="D121" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
acrécimo de quantidades vendidas no dataset
</commit_message>
<xml_diff>
--- a/produtos_precos.xlsx
+++ b/produtos_precos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,10 +446,15 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Preço de Venda</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Quantidade</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Quantidade Vendida</t>
         </is>
@@ -465,9 +470,12 @@
         <v>358</v>
       </c>
       <c r="C2" t="n">
-        <v>11</v>
+        <v>429.6</v>
       </c>
       <c r="D2" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -481,9 +489,12 @@
         <v>180</v>
       </c>
       <c r="C3" t="n">
-        <v>12</v>
+        <v>216</v>
       </c>
       <c r="D3" t="n">
+        <v>12</v>
+      </c>
+      <c r="E3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -497,9 +508,12 @@
         <v>368</v>
       </c>
       <c r="C4" t="n">
-        <v>11</v>
+        <v>441.6</v>
       </c>
       <c r="D4" t="n">
+        <v>11</v>
+      </c>
+      <c r="E4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -513,9 +527,12 @@
         <v>200</v>
       </c>
       <c r="C5" t="n">
+        <v>240</v>
+      </c>
+      <c r="D5" t="n">
         <v>13</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -529,9 +546,12 @@
         <v>71</v>
       </c>
       <c r="C6" t="n">
-        <v>11</v>
+        <v>85.2</v>
       </c>
       <c r="D6" t="n">
+        <v>11</v>
+      </c>
+      <c r="E6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -545,9 +565,12 @@
         <v>248</v>
       </c>
       <c r="C7" t="n">
-        <v>11</v>
+        <v>297.6</v>
       </c>
       <c r="D7" t="n">
+        <v>11</v>
+      </c>
+      <c r="E7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -561,9 +584,12 @@
         <v>170</v>
       </c>
       <c r="C8" t="n">
-        <v>11</v>
+        <v>204</v>
       </c>
       <c r="D8" t="n">
+        <v>11</v>
+      </c>
+      <c r="E8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -577,9 +603,12 @@
         <v>149</v>
       </c>
       <c r="C9" t="n">
+        <v>178.8</v>
+      </c>
+      <c r="D9" t="n">
         <v>14</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -593,9 +622,12 @@
         <v>116</v>
       </c>
       <c r="C10" t="n">
-        <v>11</v>
+        <v>139.2</v>
       </c>
       <c r="D10" t="n">
+        <v>11</v>
+      </c>
+      <c r="E10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -609,9 +641,12 @@
         <v>105</v>
       </c>
       <c r="C11" t="n">
-        <v>11</v>
+        <v>126</v>
       </c>
       <c r="D11" t="n">
+        <v>11</v>
+      </c>
+      <c r="E11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -625,9 +660,12 @@
         <v>706</v>
       </c>
       <c r="C12" t="n">
+        <v>847.1999999999999</v>
+      </c>
+      <c r="D12" t="n">
         <v>15</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -641,9 +679,12 @@
         <v>294</v>
       </c>
       <c r="C13" t="n">
-        <v>11</v>
+        <v>352.8</v>
       </c>
       <c r="D13" t="n">
+        <v>11</v>
+      </c>
+      <c r="E13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -657,9 +698,12 @@
         <v>259</v>
       </c>
       <c r="C14" t="n">
-        <v>12</v>
+        <v>310.8</v>
       </c>
       <c r="D14" t="n">
+        <v>12</v>
+      </c>
+      <c r="E14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -673,9 +717,12 @@
         <v>200</v>
       </c>
       <c r="C15" t="n">
-        <v>12</v>
+        <v>240</v>
       </c>
       <c r="D15" t="n">
+        <v>12</v>
+      </c>
+      <c r="E15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -689,9 +736,12 @@
         <v>69</v>
       </c>
       <c r="C16" t="n">
-        <v>11</v>
+        <v>82.8</v>
       </c>
       <c r="D16" t="n">
+        <v>11</v>
+      </c>
+      <c r="E16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -705,9 +755,12 @@
         <v>181</v>
       </c>
       <c r="C17" t="n">
-        <v>12</v>
+        <v>217.2</v>
       </c>
       <c r="D17" t="n">
+        <v>12</v>
+      </c>
+      <c r="E17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -721,9 +774,12 @@
         <v>113</v>
       </c>
       <c r="C18" t="n">
-        <v>11</v>
+        <v>135.6</v>
       </c>
       <c r="D18" t="n">
+        <v>11</v>
+      </c>
+      <c r="E18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -737,9 +793,12 @@
         <v>100</v>
       </c>
       <c r="C19" t="n">
+        <v>120</v>
+      </c>
+      <c r="D19" t="n">
         <v>14</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -753,9 +812,12 @@
         <v>114</v>
       </c>
       <c r="C20" t="n">
-        <v>12</v>
+        <v>136.8</v>
       </c>
       <c r="D20" t="n">
+        <v>12</v>
+      </c>
+      <c r="E20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -769,9 +831,12 @@
         <v>255</v>
       </c>
       <c r="C21" t="n">
-        <v>12</v>
+        <v>306</v>
       </c>
       <c r="D21" t="n">
+        <v>12</v>
+      </c>
+      <c r="E21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -785,9 +850,12 @@
         <v>218</v>
       </c>
       <c r="C22" t="n">
-        <v>11</v>
+        <v>261.6</v>
       </c>
       <c r="D22" t="n">
+        <v>11</v>
+      </c>
+      <c r="E22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -801,9 +869,12 @@
         <v>211</v>
       </c>
       <c r="C23" t="n">
-        <v>12</v>
+        <v>253.2</v>
       </c>
       <c r="D23" t="n">
+        <v>12</v>
+      </c>
+      <c r="E23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -817,9 +888,12 @@
         <v>276</v>
       </c>
       <c r="C24" t="n">
-        <v>11</v>
+        <v>331.2</v>
       </c>
       <c r="D24" t="n">
+        <v>11</v>
+      </c>
+      <c r="E24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -833,9 +907,12 @@
         <v>30</v>
       </c>
       <c r="C25" t="n">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D25" t="n">
+        <v>11</v>
+      </c>
+      <c r="E25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -849,9 +926,12 @@
         <v>78</v>
       </c>
       <c r="C26" t="n">
-        <v>12</v>
+        <v>93.59999999999999</v>
       </c>
       <c r="D26" t="n">
+        <v>12</v>
+      </c>
+      <c r="E26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -865,9 +945,12 @@
         <v>190</v>
       </c>
       <c r="C27" t="n">
-        <v>12</v>
+        <v>228</v>
       </c>
       <c r="D27" t="n">
+        <v>12</v>
+      </c>
+      <c r="E27" t="n">
         <v>0</v>
       </c>
     </row>
@@ -881,9 +964,12 @@
         <v>169</v>
       </c>
       <c r="C28" t="n">
+        <v>202.8</v>
+      </c>
+      <c r="D28" t="n">
         <v>13</v>
       </c>
-      <c r="D28" t="n">
+      <c r="E28" t="n">
         <v>0</v>
       </c>
     </row>
@@ -897,9 +983,12 @@
         <v>60</v>
       </c>
       <c r="C29" t="n">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="D29" t="n">
+        <v>12</v>
+      </c>
+      <c r="E29" t="n">
         <v>0</v>
       </c>
     </row>
@@ -913,9 +1002,12 @@
         <v>149</v>
       </c>
       <c r="C30" t="n">
-        <v>11</v>
+        <v>178.8</v>
       </c>
       <c r="D30" t="n">
+        <v>11</v>
+      </c>
+      <c r="E30" t="n">
         <v>0</v>
       </c>
     </row>
@@ -929,9 +1021,12 @@
         <v>709</v>
       </c>
       <c r="C31" t="n">
-        <v>12</v>
+        <v>850.8</v>
       </c>
       <c r="D31" t="n">
+        <v>12</v>
+      </c>
+      <c r="E31" t="n">
         <v>0</v>
       </c>
     </row>
@@ -945,9 +1040,12 @@
         <v>92</v>
       </c>
       <c r="C32" t="n">
+        <v>110.4</v>
+      </c>
+      <c r="D32" t="n">
         <v>14</v>
       </c>
-      <c r="D32" t="n">
+      <c r="E32" t="n">
         <v>0</v>
       </c>
     </row>
@@ -961,9 +1059,12 @@
         <v>256</v>
       </c>
       <c r="C33" t="n">
+        <v>307.2</v>
+      </c>
+      <c r="D33" t="n">
         <v>13</v>
       </c>
-      <c r="D33" t="n">
+      <c r="E33" t="n">
         <v>0</v>
       </c>
     </row>
@@ -977,9 +1078,12 @@
         <v>70</v>
       </c>
       <c r="C34" t="n">
+        <v>84</v>
+      </c>
+      <c r="D34" t="n">
         <v>13</v>
       </c>
-      <c r="D34" t="n">
+      <c r="E34" t="n">
         <v>0</v>
       </c>
     </row>
@@ -993,9 +1097,12 @@
         <v>124</v>
       </c>
       <c r="C35" t="n">
-        <v>11</v>
+        <v>148.8</v>
       </c>
       <c r="D35" t="n">
+        <v>11</v>
+      </c>
+      <c r="E35" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1009,9 +1116,12 @@
         <v>137</v>
       </c>
       <c r="C36" t="n">
-        <v>11</v>
+        <v>164.4</v>
       </c>
       <c r="D36" t="n">
+        <v>11</v>
+      </c>
+      <c r="E36" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1025,9 +1135,12 @@
         <v>100</v>
       </c>
       <c r="C37" t="n">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="D37" t="n">
+        <v>11</v>
+      </c>
+      <c r="E37" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1041,9 +1154,12 @@
         <v>41</v>
       </c>
       <c r="C38" t="n">
+        <v>49.2</v>
+      </c>
+      <c r="D38" t="n">
         <v>13</v>
       </c>
-      <c r="D38" t="n">
+      <c r="E38" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1057,9 +1173,12 @@
         <v>363</v>
       </c>
       <c r="C39" t="n">
-        <v>11</v>
+        <v>435.6</v>
       </c>
       <c r="D39" t="n">
+        <v>11</v>
+      </c>
+      <c r="E39" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1073,9 +1192,12 @@
         <v>118</v>
       </c>
       <c r="C40" t="n">
-        <v>12</v>
+        <v>141.6</v>
       </c>
       <c r="D40" t="n">
+        <v>12</v>
+      </c>
+      <c r="E40" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1089,9 +1211,12 @@
         <v>350</v>
       </c>
       <c r="C41" t="n">
-        <v>12</v>
+        <v>420</v>
       </c>
       <c r="D41" t="n">
+        <v>12</v>
+      </c>
+      <c r="E41" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1105,9 +1230,12 @@
         <v>37</v>
       </c>
       <c r="C42" t="n">
-        <v>11</v>
+        <v>44.4</v>
       </c>
       <c r="D42" t="n">
+        <v>11</v>
+      </c>
+      <c r="E42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1121,9 +1249,12 @@
         <v>195</v>
       </c>
       <c r="C43" t="n">
-        <v>11</v>
+        <v>234</v>
       </c>
       <c r="D43" t="n">
+        <v>11</v>
+      </c>
+      <c r="E43" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1137,9 +1268,12 @@
         <v>74</v>
       </c>
       <c r="C44" t="n">
-        <v>11</v>
+        <v>88.8</v>
       </c>
       <c r="D44" t="n">
+        <v>11</v>
+      </c>
+      <c r="E44" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1153,9 +1287,12 @@
         <v>80</v>
       </c>
       <c r="C45" t="n">
-        <v>11</v>
+        <v>96</v>
       </c>
       <c r="D45" t="n">
+        <v>11</v>
+      </c>
+      <c r="E45" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1169,9 +1306,12 @@
         <v>108</v>
       </c>
       <c r="C46" t="n">
-        <v>11</v>
+        <v>129.6</v>
       </c>
       <c r="D46" t="n">
+        <v>11</v>
+      </c>
+      <c r="E46" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1185,9 +1325,12 @@
         <v>141</v>
       </c>
       <c r="C47" t="n">
-        <v>11</v>
+        <v>169.2</v>
       </c>
       <c r="D47" t="n">
+        <v>11</v>
+      </c>
+      <c r="E47" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1201,9 +1344,12 @@
         <v>200</v>
       </c>
       <c r="C48" t="n">
-        <v>11</v>
+        <v>240</v>
       </c>
       <c r="D48" t="n">
+        <v>11</v>
+      </c>
+      <c r="E48" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1217,9 +1363,12 @@
         <v>90</v>
       </c>
       <c r="C49" t="n">
-        <v>11</v>
+        <v>108</v>
       </c>
       <c r="D49" t="n">
+        <v>11</v>
+      </c>
+      <c r="E49" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1233,9 +1382,12 @@
         <v>93</v>
       </c>
       <c r="C50" t="n">
-        <v>12</v>
+        <v>111.6</v>
       </c>
       <c r="D50" t="n">
+        <v>12</v>
+      </c>
+      <c r="E50" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1249,9 +1401,12 @@
         <v>709</v>
       </c>
       <c r="C51" t="n">
+        <v>850.8</v>
+      </c>
+      <c r="D51" t="n">
         <v>13</v>
       </c>
-      <c r="D51" t="n">
+      <c r="E51" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1265,9 +1420,12 @@
         <v>368</v>
       </c>
       <c r="C52" t="n">
-        <v>11</v>
+        <v>441.6</v>
       </c>
       <c r="D52" t="n">
+        <v>11</v>
+      </c>
+      <c r="E52" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1281,9 +1439,12 @@
         <v>214</v>
       </c>
       <c r="C53" t="n">
-        <v>11</v>
+        <v>256.8</v>
       </c>
       <c r="D53" t="n">
+        <v>11</v>
+      </c>
+      <c r="E53" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1297,9 +1458,12 @@
         <v>97</v>
       </c>
       <c r="C54" t="n">
+        <v>116.4</v>
+      </c>
+      <c r="D54" t="n">
         <v>14</v>
       </c>
-      <c r="D54" t="n">
+      <c r="E54" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1313,9 +1477,12 @@
         <v>60</v>
       </c>
       <c r="C55" t="n">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="D55" t="n">
+        <v>11</v>
+      </c>
+      <c r="E55" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1329,9 +1496,12 @@
         <v>38</v>
       </c>
       <c r="C56" t="n">
+        <v>45.6</v>
+      </c>
+      <c r="D56" t="n">
         <v>15</v>
       </c>
-      <c r="D56" t="n">
+      <c r="E56" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1345,9 +1515,12 @@
         <v>209</v>
       </c>
       <c r="C57" t="n">
-        <v>12</v>
+        <v>250.8</v>
       </c>
       <c r="D57" t="n">
+        <v>12</v>
+      </c>
+      <c r="E57" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1361,9 +1534,12 @@
         <v>299</v>
       </c>
       <c r="C58" t="n">
+        <v>358.8</v>
+      </c>
+      <c r="D58" t="n">
         <v>13</v>
       </c>
-      <c r="D58" t="n">
+      <c r="E58" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1377,9 +1553,12 @@
         <v>118</v>
       </c>
       <c r="C59" t="n">
-        <v>11</v>
+        <v>141.6</v>
       </c>
       <c r="D59" t="n">
+        <v>11</v>
+      </c>
+      <c r="E59" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1393,9 +1572,12 @@
         <v>100</v>
       </c>
       <c r="C60" t="n">
+        <v>120</v>
+      </c>
+      <c r="D60" t="n">
         <v>13</v>
       </c>
-      <c r="D60" t="n">
+      <c r="E60" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1409,9 +1591,12 @@
         <v>85</v>
       </c>
       <c r="C61" t="n">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D61" t="n">
+        <v>11</v>
+      </c>
+      <c r="E61" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1425,9 +1610,12 @@
         <v>250</v>
       </c>
       <c r="C62" t="n">
+        <v>300</v>
+      </c>
+      <c r="D62" t="n">
         <v>14</v>
       </c>
-      <c r="D62" t="n">
+      <c r="E62" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1441,9 +1629,12 @@
         <v>223</v>
       </c>
       <c r="C63" t="n">
-        <v>11</v>
+        <v>267.6</v>
       </c>
       <c r="D63" t="n">
+        <v>11</v>
+      </c>
+      <c r="E63" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1457,9 +1648,12 @@
         <v>176</v>
       </c>
       <c r="C64" t="n">
+        <v>211.2</v>
+      </c>
+      <c r="D64" t="n">
         <v>13</v>
       </c>
-      <c r="D64" t="n">
+      <c r="E64" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1473,9 +1667,12 @@
         <v>163</v>
       </c>
       <c r="C65" t="n">
-        <v>11</v>
+        <v>195.6</v>
       </c>
       <c r="D65" t="n">
+        <v>11</v>
+      </c>
+      <c r="E65" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1489,9 +1686,12 @@
         <v>750</v>
       </c>
       <c r="C66" t="n">
-        <v>12</v>
+        <v>900</v>
       </c>
       <c r="D66" t="n">
+        <v>12</v>
+      </c>
+      <c r="E66" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1505,9 +1705,12 @@
         <v>93</v>
       </c>
       <c r="C67" t="n">
-        <v>12</v>
+        <v>111.6</v>
       </c>
       <c r="D67" t="n">
+        <v>12</v>
+      </c>
+      <c r="E67" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1521,9 +1724,12 @@
         <v>67</v>
       </c>
       <c r="C68" t="n">
-        <v>11</v>
+        <v>80.39999999999999</v>
       </c>
       <c r="D68" t="n">
+        <v>11</v>
+      </c>
+      <c r="E68" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1537,9 +1743,12 @@
         <v>50</v>
       </c>
       <c r="C69" t="n">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="D69" t="n">
+        <v>12</v>
+      </c>
+      <c r="E69" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1553,9 +1762,12 @@
         <v>87</v>
       </c>
       <c r="C70" t="n">
+        <v>104.4</v>
+      </c>
+      <c r="D70" t="n">
         <v>15</v>
       </c>
-      <c r="D70" t="n">
+      <c r="E70" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1569,9 +1781,12 @@
         <v>130</v>
       </c>
       <c r="C71" t="n">
-        <v>11</v>
+        <v>156</v>
       </c>
       <c r="D71" t="n">
+        <v>11</v>
+      </c>
+      <c r="E71" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1585,9 +1800,12 @@
         <v>185</v>
       </c>
       <c r="C72" t="n">
-        <v>11</v>
+        <v>222</v>
       </c>
       <c r="D72" t="n">
+        <v>11</v>
+      </c>
+      <c r="E72" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1601,9 +1819,12 @@
         <v>187</v>
       </c>
       <c r="C73" t="n">
-        <v>11</v>
+        <v>224.4</v>
       </c>
       <c r="D73" t="n">
+        <v>11</v>
+      </c>
+      <c r="E73" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1617,9 +1838,12 @@
         <v>219</v>
       </c>
       <c r="C74" t="n">
+        <v>262.8</v>
+      </c>
+      <c r="D74" t="n">
         <v>14</v>
       </c>
-      <c r="D74" t="n">
+      <c r="E74" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1633,9 +1857,12 @@
         <v>114</v>
       </c>
       <c r="C75" t="n">
-        <v>12</v>
+        <v>136.8</v>
       </c>
       <c r="D75" t="n">
+        <v>12</v>
+      </c>
+      <c r="E75" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1649,9 +1876,12 @@
         <v>108</v>
       </c>
       <c r="C76" t="n">
+        <v>129.6</v>
+      </c>
+      <c r="D76" t="n">
         <v>15</v>
       </c>
-      <c r="D76" t="n">
+      <c r="E76" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1665,9 +1895,12 @@
         <v>215</v>
       </c>
       <c r="C77" t="n">
+        <v>258</v>
+      </c>
+      <c r="D77" t="n">
         <v>14</v>
       </c>
-      <c r="D77" t="n">
+      <c r="E77" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1681,9 +1914,12 @@
         <v>79</v>
       </c>
       <c r="C78" t="n">
-        <v>11</v>
+        <v>94.8</v>
       </c>
       <c r="D78" t="n">
+        <v>11</v>
+      </c>
+      <c r="E78" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1697,9 +1933,12 @@
         <v>87</v>
       </c>
       <c r="C79" t="n">
+        <v>104.4</v>
+      </c>
+      <c r="D79" t="n">
         <v>14</v>
       </c>
-      <c r="D79" t="n">
+      <c r="E79" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1713,9 +1952,12 @@
         <v>120</v>
       </c>
       <c r="C80" t="n">
-        <v>12</v>
+        <v>144</v>
       </c>
       <c r="D80" t="n">
+        <v>12</v>
+      </c>
+      <c r="E80" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1729,9 +1971,12 @@
         <v>311</v>
       </c>
       <c r="C81" t="n">
-        <v>12</v>
+        <v>373.2</v>
       </c>
       <c r="D81" t="n">
+        <v>12</v>
+      </c>
+      <c r="E81" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1745,9 +1990,12 @@
         <v>138</v>
       </c>
       <c r="C82" t="n">
-        <v>12</v>
+        <v>165.6</v>
       </c>
       <c r="D82" t="n">
+        <v>12</v>
+      </c>
+      <c r="E82" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1761,9 +2009,12 @@
         <v>145</v>
       </c>
       <c r="C83" t="n">
-        <v>12</v>
+        <v>174</v>
       </c>
       <c r="D83" t="n">
+        <v>12</v>
+      </c>
+      <c r="E83" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1777,9 +2028,12 @@
         <v>105</v>
       </c>
       <c r="C84" t="n">
+        <v>126</v>
+      </c>
+      <c r="D84" t="n">
         <v>13</v>
       </c>
-      <c r="D84" t="n">
+      <c r="E84" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1793,9 +2047,12 @@
         <v>277</v>
       </c>
       <c r="C85" t="n">
-        <v>11</v>
+        <v>332.4</v>
       </c>
       <c r="D85" t="n">
+        <v>11</v>
+      </c>
+      <c r="E85" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1809,9 +2066,12 @@
         <v>142</v>
       </c>
       <c r="C86" t="n">
-        <v>11</v>
+        <v>170.4</v>
       </c>
       <c r="D86" t="n">
+        <v>11</v>
+      </c>
+      <c r="E86" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1825,9 +2085,12 @@
         <v>259</v>
       </c>
       <c r="C87" t="n">
-        <v>11</v>
+        <v>310.8</v>
       </c>
       <c r="D87" t="n">
+        <v>11</v>
+      </c>
+      <c r="E87" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1841,9 +2104,12 @@
         <v>96</v>
       </c>
       <c r="C88" t="n">
-        <v>12</v>
+        <v>115.2</v>
       </c>
       <c r="D88" t="n">
+        <v>12</v>
+      </c>
+      <c r="E88" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1857,9 +2123,12 @@
         <v>66</v>
       </c>
       <c r="C89" t="n">
-        <v>11</v>
+        <v>79.2</v>
       </c>
       <c r="D89" t="n">
+        <v>11</v>
+      </c>
+      <c r="E89" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1873,9 +2142,12 @@
         <v>157</v>
       </c>
       <c r="C90" t="n">
+        <v>188.4</v>
+      </c>
+      <c r="D90" t="n">
         <v>14</v>
       </c>
-      <c r="D90" t="n">
+      <c r="E90" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1889,9 +2161,12 @@
         <v>283</v>
       </c>
       <c r="C91" t="n">
+        <v>339.6</v>
+      </c>
+      <c r="D91" t="n">
         <v>13</v>
       </c>
-      <c r="D91" t="n">
+      <c r="E91" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1905,9 +2180,12 @@
         <v>240</v>
       </c>
       <c r="C92" t="n">
-        <v>12</v>
+        <v>288</v>
       </c>
       <c r="D92" t="n">
+        <v>12</v>
+      </c>
+      <c r="E92" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1921,9 +2199,12 @@
         <v>114</v>
       </c>
       <c r="C93" t="n">
+        <v>136.8</v>
+      </c>
+      <c r="D93" t="n">
         <v>15</v>
       </c>
-      <c r="D93" t="n">
+      <c r="E93" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1937,9 +2218,12 @@
         <v>133</v>
       </c>
       <c r="C94" t="n">
-        <v>12</v>
+        <v>159.6</v>
       </c>
       <c r="D94" t="n">
+        <v>12</v>
+      </c>
+      <c r="E94" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1953,9 +2237,12 @@
         <v>391</v>
       </c>
       <c r="C95" t="n">
-        <v>12</v>
+        <v>469.2</v>
       </c>
       <c r="D95" t="n">
+        <v>12</v>
+      </c>
+      <c r="E95" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1969,9 +2256,12 @@
         <v>87</v>
       </c>
       <c r="C96" t="n">
-        <v>12</v>
+        <v>104.4</v>
       </c>
       <c r="D96" t="n">
+        <v>12</v>
+      </c>
+      <c r="E96" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1985,9 +2275,12 @@
         <v>100</v>
       </c>
       <c r="C97" t="n">
+        <v>120</v>
+      </c>
+      <c r="D97" t="n">
         <v>13</v>
       </c>
-      <c r="D97" t="n">
+      <c r="E97" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2001,9 +2294,12 @@
         <v>256</v>
       </c>
       <c r="C98" t="n">
-        <v>11</v>
+        <v>307.2</v>
       </c>
       <c r="D98" t="n">
+        <v>11</v>
+      </c>
+      <c r="E98" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2017,9 +2313,12 @@
         <v>105</v>
       </c>
       <c r="C99" t="n">
-        <v>12</v>
+        <v>126</v>
       </c>
       <c r="D99" t="n">
+        <v>12</v>
+      </c>
+      <c r="E99" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2033,9 +2332,12 @@
         <v>720</v>
       </c>
       <c r="C100" t="n">
-        <v>11</v>
+        <v>864</v>
       </c>
       <c r="D100" t="n">
+        <v>11</v>
+      </c>
+      <c r="E100" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2049,9 +2351,12 @@
         <v>266</v>
       </c>
       <c r="C101" t="n">
-        <v>11</v>
+        <v>319.2</v>
       </c>
       <c r="D101" t="n">
+        <v>11</v>
+      </c>
+      <c r="E101" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2065,9 +2370,12 @@
         <v>102</v>
       </c>
       <c r="C102" t="n">
-        <v>11</v>
+        <v>122.4</v>
       </c>
       <c r="D102" t="n">
+        <v>11</v>
+      </c>
+      <c r="E102" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2081,9 +2389,12 @@
         <v>209</v>
       </c>
       <c r="C103" t="n">
+        <v>250.8</v>
+      </c>
+      <c r="D103" t="n">
         <v>13</v>
       </c>
-      <c r="D103" t="n">
+      <c r="E103" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2097,9 +2408,12 @@
         <v>275</v>
       </c>
       <c r="C104" t="n">
+        <v>330</v>
+      </c>
+      <c r="D104" t="n">
         <v>13</v>
       </c>
-      <c r="D104" t="n">
+      <c r="E104" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2113,9 +2427,12 @@
         <v>270</v>
       </c>
       <c r="C105" t="n">
+        <v>324</v>
+      </c>
+      <c r="D105" t="n">
         <v>13</v>
       </c>
-      <c r="D105" t="n">
+      <c r="E105" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2129,9 +2446,12 @@
         <v>155</v>
       </c>
       <c r="C106" t="n">
-        <v>12</v>
+        <v>186</v>
       </c>
       <c r="D106" t="n">
+        <v>12</v>
+      </c>
+      <c r="E106" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2145,9 +2465,12 @@
         <v>216</v>
       </c>
       <c r="C107" t="n">
+        <v>259.2</v>
+      </c>
+      <c r="D107" t="n">
         <v>13</v>
       </c>
-      <c r="D107" t="n">
+      <c r="E107" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2161,9 +2484,12 @@
         <v>262</v>
       </c>
       <c r="C108" t="n">
+        <v>314.4</v>
+      </c>
+      <c r="D108" t="n">
         <v>13</v>
       </c>
-      <c r="D108" t="n">
+      <c r="E108" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2177,9 +2503,12 @@
         <v>700</v>
       </c>
       <c r="C109" t="n">
+        <v>840</v>
+      </c>
+      <c r="D109" t="n">
         <v>15</v>
       </c>
-      <c r="D109" t="n">
+      <c r="E109" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2193,9 +2522,12 @@
         <v>250</v>
       </c>
       <c r="C110" t="n">
-        <v>12</v>
+        <v>300</v>
       </c>
       <c r="D110" t="n">
+        <v>12</v>
+      </c>
+      <c r="E110" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2209,9 +2541,12 @@
         <v>177</v>
       </c>
       <c r="C111" t="n">
+        <v>212.4</v>
+      </c>
+      <c r="D111" t="n">
         <v>13</v>
       </c>
-      <c r="D111" t="n">
+      <c r="E111" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2225,9 +2560,12 @@
         <v>197</v>
       </c>
       <c r="C112" t="n">
+        <v>236.4</v>
+      </c>
+      <c r="D112" t="n">
         <v>13</v>
       </c>
-      <c r="D112" t="n">
+      <c r="E112" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2241,9 +2579,12 @@
         <v>50</v>
       </c>
       <c r="C113" t="n">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="D113" t="n">
+        <v>11</v>
+      </c>
+      <c r="E113" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2257,9 +2598,12 @@
         <v>196</v>
       </c>
       <c r="C114" t="n">
-        <v>11</v>
+        <v>235.2</v>
       </c>
       <c r="D114" t="n">
+        <v>11</v>
+      </c>
+      <c r="E114" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2273,9 +2617,12 @@
         <v>150</v>
       </c>
       <c r="C115" t="n">
-        <v>12</v>
+        <v>180</v>
       </c>
       <c r="D115" t="n">
+        <v>12</v>
+      </c>
+      <c r="E115" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2289,9 +2636,12 @@
         <v>214</v>
       </c>
       <c r="C116" t="n">
-        <v>11</v>
+        <v>256.8</v>
       </c>
       <c r="D116" t="n">
+        <v>11</v>
+      </c>
+      <c r="E116" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2305,9 +2655,12 @@
         <v>107</v>
       </c>
       <c r="C117" t="n">
-        <v>11</v>
+        <v>128.4</v>
       </c>
       <c r="D117" t="n">
+        <v>11</v>
+      </c>
+      <c r="E117" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2321,9 +2674,12 @@
         <v>66</v>
       </c>
       <c r="C118" t="n">
+        <v>79.2</v>
+      </c>
+      <c r="D118" t="n">
         <v>13</v>
       </c>
-      <c r="D118" t="n">
+      <c r="E118" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2337,9 +2693,12 @@
         <v>269</v>
       </c>
       <c r="C119" t="n">
-        <v>11</v>
+        <v>322.8</v>
       </c>
       <c r="D119" t="n">
+        <v>11</v>
+      </c>
+      <c r="E119" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2353,9 +2712,12 @@
         <v>73</v>
       </c>
       <c r="C120" t="n">
-        <v>12</v>
+        <v>87.59999999999999</v>
       </c>
       <c r="D120" t="n">
+        <v>12</v>
+      </c>
+      <c r="E120" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2369,9 +2731,12 @@
         <v>116</v>
       </c>
       <c r="C121" t="n">
+        <v>139.2</v>
+      </c>
+      <c r="D121" t="n">
         <v>13</v>
       </c>
-      <c r="D121" t="n">
+      <c r="E121" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>